<commit_message>
The main change is how the patterns are written to the nodes.   Also corrected the selected patterns based on the current view mode (patterns vs nodes) and correctly save the restore parameters after transferring the patterns.
git-svn-id: https://jdc-consulting.unfuddle.com/svn/jdc-consulting_matlabapi@252 03bc5d11-0c36-4e61-bad9-4efbbe88aa87
</commit_message>
<xml_diff>
--- a/trunk/apps/Reference/PatternTemplates.xlsx
+++ b/trunk/apps/Reference/PatternTemplates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhart\Documents\MATLAB\NNP\NNPAPI\trunk\apps\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FC67BD-E5FF-4DE1-8CDB-A2AD33643289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A57DF8-6946-4596-9818-6ACF0B91D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="14790" xr2:uid="{7D8F7F71-9B30-4A8F-85E5-70580157DEDE}"/>
+    <workbookView xWindow="-42945" yWindow="-6390" windowWidth="37395" windowHeight="17940" activeTab="7" xr2:uid="{7D8F7F71-9B30-4A8F-85E5-70580157DEDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lateral FF" sheetId="9" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Palmar Power" sheetId="5" r:id="rId5"/>
     <sheet name="Palmar Light" sheetId="7" r:id="rId6"/>
     <sheet name="Triceps" sheetId="8" r:id="rId7"/>
+    <sheet name="Exercise NoThContact" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="30">
   <si>
     <t>Muscle Type</t>
   </si>
@@ -120,6 +121,15 @@
   </si>
   <si>
     <t>MuscleType</t>
+  </si>
+  <si>
+    <t>Exercise with No Thumb Contact</t>
+  </si>
+  <si>
+    <t>Plots generated in separate file, Pattern Plots for Templates Rev N.xlsx</t>
+  </si>
+  <si>
+    <t>That allows better spacing and muscle name examples</t>
   </si>
 </sst>
 </file>
@@ -612,6 +622,61 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>5442</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1018</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D04D438E-1C73-ED98-DE26-03FC2BC209D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7119256" y="234044"/>
+          <a:ext cx="4615543" cy="3386474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -909,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F4B4BF-51B9-4681-B8D6-0D52D92B1E92}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1419,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -1435,12 +1500,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1463,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5690F366-E097-4422-8872-7E138A36FC95}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L23" sqref="L23:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1973,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1981,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -1989,12 +2062,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2017,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DBE92E-FD65-41F5-A94F-844F369722EC}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:A1048576"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2495,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2527,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2535,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2543,12 +2626,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2571,10 +2664,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E945C10E-7F58-4AA3-AC5D-AA672EE7A4D6}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L22" sqref="L22:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3081,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -3089,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -3097,12 +3190,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3149,10 +3250,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FA643F-9C96-4BB6-B22F-D30595C3BEDF}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L22" sqref="L22:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3627,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3659,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -3667,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -3675,12 +3776,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3703,10 +3812,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF2C659-4AAA-433A-BA7D-0A0B3AED48B4}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L22" sqref="L22:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4181,7 +4290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4213,7 +4322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -4221,7 +4330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -4229,12 +4338,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -4257,10 +4374,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6288E2F-E183-4EA9-99D0-8494CBEF2813}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A17"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4735,7 +4852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4767,7 +4884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -4775,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -4783,12 +4900,584 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B5:J17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color theme="0"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF835E55-00DF-4C7D-AB3F-1455464AAE95}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>64</v>
+      </c>
+      <c r="E3" s="4">
+        <v>96</v>
+      </c>
+      <c r="F3" s="4">
+        <v>128</v>
+      </c>
+      <c r="G3" s="4">
+        <v>160</v>
+      </c>
+      <c r="H3" s="4">
+        <v>192</v>
+      </c>
+      <c r="I3" s="4">
+        <v>224</v>
+      </c>
+      <c r="J3" s="4">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>